<commit_message>
feat: new measurement forms
</commit_message>
<xml_diff>
--- a/data/punts/harnser-51-sail-measurement.xlsx
+++ b/data/punts/harnser-51-sail-measurement.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Invate\Documents\DIcks Docs\Punt\Measurement Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Invate\Documents\DIcks Docs\Punt\Measurement Forms\Current forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{055529D6-F017-44E4-A3E4-606432706DC7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="6" r:id="rId1"/>
@@ -515,7 +516,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1729,7 +1730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2045,7 +2046,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2081,7 +2082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:J140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2415,7 +2416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2515,7 +2516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2540,11 +2541,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,7 +2608,7 @@
         <v>138</v>
       </c>
       <c r="C8" s="37">
-        <v>7447</v>
+        <v>7423</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -2615,7 +2616,7 @@
         <v>139</v>
       </c>
       <c r="C9" s="39">
-        <v>2727</v>
+        <v>2598</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2623,7 +2624,7 @@
         <v>140</v>
       </c>
       <c r="C10" s="40">
-        <v>7898</v>
+        <v>7836</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2667,13 +2668,13 @@
         <v>6</v>
       </c>
       <c r="C13" s="35">
-        <v>7898</v>
+        <v>7836</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="35">
-        <v>2579</v>
+        <v>2459</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>2</v>
@@ -2687,7 +2688,7 @@
       </c>
       <c r="I13" s="6">
         <f>C13*E13*G13</f>
-        <v>10184471</v>
+        <v>9634362</v>
       </c>
       <c r="J13" s="27" t="s">
         <v>128</v>
@@ -2698,13 +2699,13 @@
         <v>7</v>
       </c>
       <c r="C14" s="36">
-        <v>7447</v>
+        <v>7423</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="36">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>2</v>
@@ -2718,7 +2719,7 @@
       </c>
       <c r="I14" s="6">
         <f t="shared" ref="I14:I43" si="1">C14*E14*G14</f>
-        <v>680162.73413</v>
+        <v>554253.43791999994</v>
       </c>
       <c r="J14" s="27" t="s">
         <v>128</v>
@@ -2726,30 +2727,30 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="36">
-        <v>2727</v>
+        <v>2598</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="36">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>0.66667</v>
+        <v>0.5</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I15" s="6">
         <f t="shared" si="1"/>
-        <v>201799.00899</v>
+        <v>161076</v>
       </c>
       <c r="J15" s="27" t="s">
         <v>128</v>
@@ -2760,13 +2761,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="36">
-        <v>7898</v>
+        <v>7836</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="36">
-        <v>700</v>
+        <v>1019</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>2</v>
@@ -2780,7 +2781,7 @@
       </c>
       <c r="I16" s="6">
         <f t="shared" si="1"/>
-        <v>2764300</v>
+        <v>3992442</v>
       </c>
       <c r="J16" s="27" t="s">
         <v>128</v>
@@ -2788,30 +2789,30 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="36">
-        <v>4529</v>
+        <v>1625</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="36">
-        <v>98</v>
+        <v>645</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>0.66667</v>
+        <v>0.5</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I17" s="6">
         <f t="shared" si="1"/>
-        <v>295896.14613999997</v>
+        <v>524062.5</v>
       </c>
       <c r="J17" s="27" t="s">
         <v>128</v>
@@ -2819,30 +2820,30 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="42" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" s="36">
-        <v>3493</v>
+        <v>6641</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="36">
-        <v>388</v>
+        <v>55</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.66667</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I18" s="6">
         <f t="shared" si="1"/>
-        <v>677642</v>
+        <v>243504.55085</v>
       </c>
       <c r="J18" s="27" t="s">
         <v>128</v>
@@ -2850,30 +2851,26 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="36">
-        <v>2728</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C19" s="36"/>
       <c r="D19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="36">
-        <v>115</v>
-      </c>
+      <c r="E19" s="36"/>
       <c r="F19" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>0.66667</v>
+        <v>0.5</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I19" s="6">
         <f t="shared" si="1"/>
-        <v>209147.71239999999</v>
+        <v>0</v>
       </c>
       <c r="J19" s="27" t="s">
         <v>128</v>
@@ -2883,15 +2880,11 @@
       <c r="B20" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="36">
-        <v>8756</v>
-      </c>
+      <c r="C20" s="36"/>
       <c r="D20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="36">
-        <v>60</v>
-      </c>
+      <c r="E20" s="36"/>
       <c r="F20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2904,7 +2897,7 @@
       </c>
       <c r="I20" s="6">
         <f t="shared" ref="I20:I24" si="3">C20*E20*G20</f>
-        <v>262680</v>
+        <v>0</v>
       </c>
       <c r="J20" s="27" t="s">
         <v>128</v>
@@ -3487,7 +3480,7 @@
       </c>
       <c r="I44" s="13">
         <f>I13+I14+I15+I16+I17+I18+I19+I20+I21+I22+I23+I24+I25+I26+I27+I28+I29+I30+I31+I32-I34-I35-I36-I37-I38-I39-I40-I41-I42-I43</f>
-        <v>15276098.60166</v>
+        <v>15109700.488770001</v>
       </c>
       <c r="J44" s="16"/>
     </row>
@@ -3982,7 +3975,7 @@
       </c>
       <c r="C69" s="18">
         <f>I44/1000000</f>
-        <v>15.276098601659999</v>
+        <v>15.109700488770001</v>
       </c>
     </row>
     <row r="70" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4000,7 +3993,7 @@
       </c>
       <c r="C71" s="25">
         <f>C69+C70</f>
-        <v>21.718494851700001</v>
+        <v>21.55209673881</v>
       </c>
     </row>
     <row r="72" spans="2:10" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -4032,7 +4025,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
             <xm:f>Formatting!$A$1:$A$2</xm:f>
           </x14:formula1>
@@ -4045,7 +4038,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4057,7 +4050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>